<commit_message>
se arregló el error con el item PantallaInicio, esto afectpo el recording Personas.rxrec Se modif los Datasources para hacer la regre en PreProd R30
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP Enlatada.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3C527-3494-4157-9E62-5FA5A0DBCAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B61C85F-6EEE-4473-A5C2-1E70D50A150A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -111,16 +112,16 @@
     <t>81 ver. 2</t>
   </si>
   <si>
-    <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
-  </si>
-  <si>
-    <t>i-preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
 </sst>
 </file>
@@ -458,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,10 +526,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -537,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2">
-        <v>8847544113</v>
+        <v>5746832029</v>
       </c>
       <c r="F2">
         <v>2344</v>
@@ -561,153 +562,170 @@
         <v>16</v>
       </c>
       <c r="N2">
-        <v>30990133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>1143792935</v>
-      </c>
-      <c r="F4">
-        <v>2344</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4">
-        <v>27990130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1143792935</v>
-      </c>
-      <c r="F5">
-        <v>2344</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5">
-        <v>26990134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>8965431747</v>
-      </c>
-      <c r="F6">
-        <v>2344</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6">
-        <v>26990138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
+        <v>30990134</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{012B90AE-69C9-4456-B396-03AA009029BA}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{8DA4B6B7-683B-42E0-AECF-0F585469EC0B}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{9FCC594A-5246-4343-908B-B2FE8ED64BD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D763992D-3DC7-4A0F-BB9F-64006EAF1C66}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>1143792935</v>
+      </c>
+      <c r="F1">
+        <v>2344</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1">
+        <v>27990130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1143792935</v>
+      </c>
+      <c r="F2">
+        <v>2344</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>26990134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>8965431747</v>
+      </c>
+      <c r="F3">
+        <v>2344</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>26990138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{012B90AE-69C9-4456-B396-03AA009029BA}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8DA4B6B7-683B-42E0-AECF-0F585469EC0B}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{9FCC594A-5246-4343-908B-B2FE8ED64BD0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se sube nueva data para regresion en preProd
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B61C85F-6EEE-4473-A5C2-1E70D50A150A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F72C7B7-C74E-4C13-9EDB-CBAECF43BC9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2">
-        <v>5746832029</v>
+        <v>3199801311</v>
       </c>
       <c r="F2">
         <v>2344</v>
@@ -562,7 +562,7 @@
         <v>16</v>
       </c>
       <c r="N2">
-        <v>30990134</v>
+        <v>30990137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modificaron las cuentas de todos los datasources
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C25777-6333-4E9D-937E-6C5CFB71E67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E114C1FC-FCB2-4AB2-B8FA-904D0BFFD99B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2">
-        <v>3199801311</v>
+        <v>7145989545</v>
       </c>
       <c r="F2">
         <v>2344</v>
@@ -582,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="2">
-        <v>3199801311</v>
+        <v>7145989545</v>
       </c>
       <c r="F3">
         <v>2344</v>

</xml_diff>

<commit_message>
se modificad data para regresion en preprod R33
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E114C1FC-FCB2-4AB2-B8FA-904D0BFFD99B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE02531-2EFC-4D87-8895-D997973C854A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2">
-        <v>7145989545</v>
+        <v>7068873718</v>
       </c>
       <c r="F2">
         <v>2344</v>
@@ -582,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="2">
-        <v>7145989545</v>
+        <v>7068873718</v>
       </c>
       <c r="F3">
         <v>2344</v>

</xml_diff>